<commit_message>
updated exports and results
</commit_message>
<xml_diff>
--- a/experiments/2022_car_sampling_pnec/results/sample_time_results.xlsx
+++ b/experiments/2022_car_sampling_pnec/results/sample_time_results.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
   <si>
     <t>sample</t>
   </si>
@@ -56,19 +56,19 @@
     <t>AW &amp; ST: Selfreport (w/ App)</t>
   </si>
   <si>
+    <t>AW: Sensor, ST: Selfreport (w/o App)</t>
+  </si>
+  <si>
+    <t>AW: Sensor, ST: Selfreport (w/ App)</t>
+  </si>
+  <si>
+    <t>AW: Sensor, ST: App</t>
+  </si>
+  <si>
+    <t>cum_sampling_delay</t>
+  </si>
+  <si>
     <t>AW &amp; ST: App</t>
-  </si>
-  <si>
-    <t>AW: Sensor, ST: Selfreport (w/o App)</t>
-  </si>
-  <si>
-    <t>AW: Sensor, ST: Selfreport (w/ App)</t>
-  </si>
-  <si>
-    <t>AW: Sensor, ST: App</t>
-  </si>
-  <si>
-    <t>cum_sampling_delay</t>
   </si>
   <si>
     <t>AW &amp; ST: Selfreport</t>
@@ -471,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -617,34 +617,34 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.9399999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="C6">
-        <v>1.18</v>
+        <v>3.03</v>
       </c>
       <c r="D6">
-        <v>1.49</v>
+        <v>4.35</v>
       </c>
       <c r="E6">
-        <v>1.51</v>
+        <v>2.88</v>
       </c>
       <c r="F6">
-        <v>2.03</v>
+        <v>5.07</v>
       </c>
       <c r="G6">
-        <v>1.78</v>
+        <v>3.12</v>
       </c>
       <c r="H6">
-        <v>2.47</v>
+        <v>5.4</v>
       </c>
       <c r="I6">
-        <v>2.05</v>
+        <v>3.38</v>
       </c>
       <c r="J6">
-        <v>2.92</v>
+        <v>5.43</v>
       </c>
       <c r="K6">
-        <v>2.15</v>
+        <v>3.43</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -652,34 +652,34 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>3.9</v>
+        <v>3.76</v>
       </c>
       <c r="C7">
-        <v>3.03</v>
+        <v>2.68</v>
       </c>
       <c r="D7">
-        <v>4.35</v>
+        <v>3.79</v>
       </c>
       <c r="E7">
-        <v>2.88</v>
+        <v>2.78</v>
       </c>
       <c r="F7">
-        <v>5.07</v>
+        <v>4.62</v>
       </c>
       <c r="G7">
-        <v>3.12</v>
+        <v>2.73</v>
       </c>
       <c r="H7">
-        <v>5.4</v>
+        <v>5.18</v>
       </c>
       <c r="I7">
-        <v>3.38</v>
+        <v>3.15</v>
       </c>
       <c r="J7">
-        <v>5.43</v>
+        <v>5.52</v>
       </c>
       <c r="K7">
-        <v>3.43</v>
+        <v>3.05</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -687,68 +687,33 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>3.76</v>
+        <v>4.34</v>
       </c>
       <c r="C8">
-        <v>2.68</v>
+        <v>1.93</v>
       </c>
       <c r="D8">
-        <v>3.79</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>2.78</v>
+        <v>2.1</v>
       </c>
       <c r="F8">
-        <v>4.62</v>
+        <v>5.68</v>
       </c>
       <c r="G8">
-        <v>2.73</v>
+        <v>2.59</v>
       </c>
       <c r="H8">
-        <v>5.18</v>
+        <v>6.16</v>
       </c>
       <c r="I8">
-        <v>3.15</v>
+        <v>2.61</v>
       </c>
       <c r="J8">
-        <v>5.52</v>
+        <v>6.63</v>
       </c>
       <c r="K8">
-        <v>3.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>4.34</v>
-      </c>
-      <c r="C9">
-        <v>1.93</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <v>2.1</v>
-      </c>
-      <c r="F9">
-        <v>5.68</v>
-      </c>
-      <c r="G9">
-        <v>2.59</v>
-      </c>
-      <c r="H9">
-        <v>6.16</v>
-      </c>
-      <c r="I9">
-        <v>2.61</v>
-      </c>
-      <c r="J9">
-        <v>6.63</v>
-      </c>
-      <c r="K9">
         <v>2.77</v>
       </c>
     </row>
@@ -766,7 +731,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -775,7 +740,7 @@
     <row r="1" spans="1:3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -820,10 +785,10 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>1.66</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1.58</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -831,10 +796,10 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -842,20 +807,9 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>1.99</v>
       </c>
       <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>1.99</v>
-      </c>
-      <c r="C9">
         <v>1.64</v>
       </c>
     </row>
@@ -905,31 +859,31 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>17</v>
@@ -1114,7 +1068,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>96.25</v>
@@ -1160,7 +1114,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>65.84999999999999</v>
@@ -1171,7 +1125,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>60.78</v>

</xml_diff>

<commit_message>
updated notebooks and outputs
</commit_message>
<xml_diff>
--- a/experiments/2022_car_sampling_pnec/results/sample_time_results.xlsx
+++ b/experiments/2022_car_sampling_pnec/results/sample_time_results.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
   <si>
     <t>sample</t>
   </si>
@@ -56,6 +56,9 @@
     <t>AW &amp; ST: Selfreport (w/ App)</t>
   </si>
   <si>
+    <t>AW &amp; ST: App</t>
+  </si>
+  <si>
     <t>AW: Sensor, ST: Selfreport (w/o App)</t>
   </si>
   <si>
@@ -66,9 +69,6 @@
   </si>
   <si>
     <t>cum_sampling_delay</t>
-  </si>
-  <si>
-    <t>AW &amp; ST: App</t>
   </si>
   <si>
     <t>AW &amp; ST: Selfreport</t>
@@ -471,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -617,34 +617,34 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>3.9</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C6">
-        <v>3.03</v>
+        <v>1.18</v>
       </c>
       <c r="D6">
-        <v>4.35</v>
+        <v>1.49</v>
       </c>
       <c r="E6">
-        <v>2.88</v>
+        <v>1.51</v>
       </c>
       <c r="F6">
-        <v>5.07</v>
+        <v>2.03</v>
       </c>
       <c r="G6">
-        <v>3.12</v>
+        <v>1.78</v>
       </c>
       <c r="H6">
-        <v>5.4</v>
+        <v>2.47</v>
       </c>
       <c r="I6">
-        <v>3.38</v>
+        <v>2.05</v>
       </c>
       <c r="J6">
-        <v>5.43</v>
+        <v>2.92</v>
       </c>
       <c r="K6">
-        <v>3.43</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -652,34 +652,34 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>3.76</v>
+        <v>3.9</v>
       </c>
       <c r="C7">
-        <v>2.68</v>
+        <v>3.03</v>
       </c>
       <c r="D7">
-        <v>3.79</v>
+        <v>4.35</v>
       </c>
       <c r="E7">
-        <v>2.78</v>
+        <v>2.88</v>
       </c>
       <c r="F7">
-        <v>4.62</v>
+        <v>5.07</v>
       </c>
       <c r="G7">
-        <v>2.73</v>
+        <v>3.12</v>
       </c>
       <c r="H7">
-        <v>5.18</v>
+        <v>5.4</v>
       </c>
       <c r="I7">
-        <v>3.15</v>
+        <v>3.38</v>
       </c>
       <c r="J7">
-        <v>5.52</v>
+        <v>5.43</v>
       </c>
       <c r="K7">
-        <v>3.05</v>
+        <v>3.43</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -687,33 +687,68 @@
         <v>14</v>
       </c>
       <c r="B8">
+        <v>3.76</v>
+      </c>
+      <c r="C8">
+        <v>2.68</v>
+      </c>
+      <c r="D8">
+        <v>3.79</v>
+      </c>
+      <c r="E8">
+        <v>2.78</v>
+      </c>
+      <c r="F8">
+        <v>4.62</v>
+      </c>
+      <c r="G8">
+        <v>2.73</v>
+      </c>
+      <c r="H8">
+        <v>5.18</v>
+      </c>
+      <c r="I8">
+        <v>3.15</v>
+      </c>
+      <c r="J8">
+        <v>5.52</v>
+      </c>
+      <c r="K8">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
         <v>4.34</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>1.93</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>5</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>2.1</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>5.68</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>2.59</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>6.16</v>
       </c>
-      <c r="I8">
+      <c r="I9">
         <v>2.61</v>
       </c>
-      <c r="J8">
+      <c r="J9">
         <v>6.63</v>
       </c>
-      <c r="K8">
+      <c r="K9">
         <v>2.77</v>
       </c>
     </row>
@@ -731,7 +766,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -740,7 +775,7 @@
     <row r="1" spans="1:3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -785,10 +820,10 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1.66</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -796,10 +831,10 @@
         <v>13</v>
       </c>
       <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>1</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -807,9 +842,20 @@
         <v>14</v>
       </c>
       <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
         <v>1.99</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>1.64</v>
       </c>
     </row>
@@ -859,31 +905,31 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>17</v>
@@ -1068,7 +1114,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>96.25</v>
@@ -1114,7 +1160,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>65.84999999999999</v>
@@ -1125,7 +1171,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>60.78</v>

</xml_diff>